<commit_message>
Changed R2 LED-B-GPIO2 resistor from 10k to 33k for correct boot in KiCad project and excel production files. Added semafor riddle mode.
</commit_message>
<xml_diff>
--- a/ele/semaforBoard/Fabrication/panel1-bom.xlsx
+++ b/ele/semaforBoard/Fabrication/panel1-bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robotarna\Semafor\ele\semaforBoard\Fabrication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA49561-477B-4AAE-BD69-30FB726802BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17F8768-315B-4BC3-A7AA-B46BE8B82C34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{35FB70B8-7432-47C9-A778-25680847F295}"/>
+    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{35FB70B8-7432-47C9-A778-25680847F295}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Designator</t>
   </si>
@@ -58,9 +58,6 @@
     <t>CH340G</t>
   </si>
   <si>
-    <t>R10,R4,R3,R2,R1,R10,R4,R3,R2,R1,R10,R4,R3,R2,R1,R10,R4,R3,R2,R1</t>
-  </si>
-  <si>
     <t>R_1206_3216Metric_Pad1.42x1.75mm_HandSolder</t>
   </si>
   <si>
@@ -152,6 +149,18 @@
   </si>
   <si>
     <t>39R</t>
+  </si>
+  <si>
+    <t>33k</t>
+  </si>
+  <si>
+    <t>R2,R2,R2,R2</t>
+  </si>
+  <si>
+    <t>C18004</t>
+  </si>
+  <si>
+    <t>R10,R4,R3,R1,R10,R4,R3,R1,R10,R4,R3,R1,R10,R4,R3,R1</t>
   </si>
 </sst>
 </file>
@@ -205,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -213,6 +222,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D0FBB9-C64E-45B4-B7E3-CBC48D4EB174}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,16 +554,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -569,7 +580,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1">
         <v>4</v>
@@ -577,16 +588,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2">
         <v>20</v>
@@ -594,16 +605,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1">
         <v>20</v>
@@ -611,16 +622,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2">
         <v>8</v>
@@ -628,16 +639,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1">
         <v>8</v>
@@ -645,16 +656,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2">
         <v>4</v>
@@ -662,16 +673,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1">
         <v>8</v>
@@ -679,16 +690,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2">
         <v>8</v>
@@ -696,18 +707,35 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="B11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="8">
         <v>4</v>
       </c>
     </row>

</xml_diff>